<commit_message>
Add scenarios for PDE file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/MFP-tests.xlsx
+++ b/src/test/resources/testData/MFP-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rachowdhury\Documents\Software\mtf-automation-testing-api\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF229C5-AD18-4458-AED2-BA51881A0A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F5FBCA-7DB2-444C-9363-7766AEDFEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>test_case_id</t>
   </si>
@@ -59,6 +59,27 @@
   </si>
   <si>
     <t xml:space="preserve"> select ndc_eleven from mfp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select ndc_eleven, effective_date from mfp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getFromFile("ndc_eleven", "effective_date")</t>
+  </si>
+  <si>
+    <t>Test NDC-11 and Effective Date Dynamicly</t>
+  </si>
+  <si>
+    <t>{
+	{ 
+		"ndc_eleven": "00003-0893-21",
+		"effective-date": "1/1/2026"
+	},
+	{
+		"ndc_eleven": "00003-0893-31",
+		"effective_date": "1/1/2026"
+	}
+}</t>
   </si>
 </sst>
 </file>
@@ -542,8 +563,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -899,18 +923,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.21875" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -973,7 +997,36 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="256.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ready to discuss assignable tasks for File Handler
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/MFP-tests.xlsx
+++ b/src/test/resources/testData/MFP-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rachowdhury\Documents\Software\mtf-automation-testing-api\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F5FBCA-7DB2-444C-9363-7766AEDFEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452896B7-9B06-4F1C-ACA4-5267BDBB6894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> insulin, tylenol, vaccine</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Count all rows</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
 		"effective_date": "1/1/2026"
 	}
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> APIXABAN, ETANERCEPT</t>
   </si>
 </sst>
 </file>
@@ -957,13 +957,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -974,10 +974,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>32</v>
@@ -988,13 +988,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="256.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1002,13 +1002,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1016,13 +1016,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>